<commit_message>
2019.07.22.Mon. 22:59 Edited The Doc of Git by stone.
</commit_message>
<xml_diff>
--- a/GitGitHubSVN.xlsx
+++ b/GitGitHubSVN.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
   <si>
     <t>작업이력</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -464,6 +464,10 @@
   </si>
   <si>
     <t xml:space="preserve">#4. 팀의 작업 진척 상황 확인 </t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>GitHub 계정을 만들고, 파일을 올린다. (Push) - 크롬에서 Octotree 를 설치하면 왼쪽에 탐색기처럼 나타난다.</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
@@ -1502,14 +1506,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>237066</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>160865</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>226591</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>220133</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>209658</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>110198</xdr:rowOff>
     </xdr:to>
@@ -1520,8 +1524,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8131386" y="160865"/>
-          <a:ext cx="1110827" cy="284613"/>
+          <a:off x="4798591" y="160865"/>
+          <a:ext cx="1126067" cy="266833"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout2">
           <a:avLst>
@@ -1577,14 +1581,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>36687</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>160865</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>26212</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>19754</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>9279</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>110198</xdr:rowOff>
     </xdr:to>
@@ -1595,8 +1599,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9340707" y="160865"/>
-          <a:ext cx="1110827" cy="284613"/>
+          <a:off x="6026962" y="160865"/>
+          <a:ext cx="1126067" cy="266833"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout2">
           <a:avLst>
@@ -1652,14 +1656,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>115708</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>160865</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>105233</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>98775</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>88300</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>110198</xdr:rowOff>
     </xdr:to>
@@ -1670,8 +1674,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10547488" y="160865"/>
-          <a:ext cx="1110827" cy="284613"/>
+          <a:off x="7248983" y="160865"/>
+          <a:ext cx="1126067" cy="266833"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout2">
           <a:avLst>
@@ -1727,14 +1731,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>194728</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>160865</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>184253</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>177795</xdr:colOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>167320</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>110198</xdr:rowOff>
     </xdr:to>
@@ -1745,8 +1749,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11754268" y="160865"/>
-          <a:ext cx="1110827" cy="284613"/>
+          <a:off x="8471003" y="160865"/>
+          <a:ext cx="1126067" cy="266833"/>
         </a:xfrm>
         <a:prstGeom prst="borderCallout2">
           <a:avLst>
@@ -1802,14 +1806,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>245534</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>235059</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>160867</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>150392</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1590</xdr:rowOff>
     </xdr:to>
@@ -1820,8 +1824,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8139854" y="701042"/>
-          <a:ext cx="1043093" cy="1588"/>
+          <a:off x="4807059" y="645585"/>
+          <a:ext cx="1058333" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1853,14 +1857,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>70559</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>60084</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>265292</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>254817</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1590</xdr:rowOff>
     </xdr:to>
@@ -1871,8 +1875,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9374579" y="701042"/>
-          <a:ext cx="1040553" cy="1588"/>
+          <a:off x="6060834" y="645585"/>
+          <a:ext cx="1051983" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1904,14 +1908,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>174984</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>164509</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>41</xdr:col>
-      <xdr:colOff>90317</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>79842</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1590</xdr:rowOff>
     </xdr:to>
@@ -1922,8 +1926,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10606764" y="701042"/>
-          <a:ext cx="1043093" cy="1588"/>
+          <a:off x="7308259" y="645585"/>
+          <a:ext cx="1058333" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1955,14 +1959,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>8</xdr:colOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>275283</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>2</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>194741</xdr:colOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>184266</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1590</xdr:rowOff>
     </xdr:to>
@@ -1973,8 +1977,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11841488" y="701042"/>
-          <a:ext cx="1040553" cy="1588"/>
+          <a:off x="8562033" y="645585"/>
+          <a:ext cx="1051983" cy="1588"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2006,13 +2010,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>78</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>264583</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>81</xdr:col>
+      <xdr:col>40</xdr:col>
       <xdr:colOff>127333</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>32083</xdr:rowOff>
@@ -2044,13 +2048,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>82</xdr:col>
+      <xdr:col>41</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>115</xdr:col>
+      <xdr:col>74</xdr:col>
       <xdr:colOff>246441</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>28667</xdr:rowOff>
@@ -3100,6 +3104,44 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>76</xdr:col>
+      <xdr:colOff>189227</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>112763</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="그림 31" descr="601_github.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11715750" y="9884833"/>
+          <a:ext cx="10190477" cy="12304763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3804,12 +3846,12 @@
   <sheetPr>
     <tabColor rgb="FFFFFFCC"/>
   </sheetPr>
-  <dimension ref="B1:CE136"/>
+  <dimension ref="B1:AP136"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AM30" sqref="AM30"/>
-      <selection pane="bottomLeft" activeCell="N62" sqref="N62"/>
+      <selection pane="bottomLeft" activeCell="AP58" sqref="AP58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.75" defaultRowHeight="13.5"/>
@@ -3817,7 +3859,7 @@
     <col min="1" max="16384" width="3.75" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:83" s="17" customFormat="1" ht="12.75">
+    <row r="1" spans="2:42" s="17" customFormat="1" ht="12.75">
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
@@ -3828,19 +3870,8 @@
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
-      <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="1"/>
-      <c r="AN1" s="1"/>
-      <c r="AO1" s="1"/>
-      <c r="AP1" s="1"/>
-      <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-    </row>
-    <row r="2" spans="2:83" s="17" customFormat="1" ht="12.75">
+    </row>
+    <row r="2" spans="2:42" s="17" customFormat="1" ht="12.75">
       <c r="B2" s="17" t="s">
         <v>21</v>
       </c>
@@ -3854,22 +3885,11 @@
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
-      <c r="AN2" s="1"/>
-      <c r="AO2" s="1"/>
-      <c r="AP2" s="1"/>
-      <c r="AQ2" s="1"/>
-      <c r="AR2" s="1"/>
-      <c r="AS2" s="1"/>
-      <c r="AT2" s="1"/>
-      <c r="AU2" s="1"/>
-      <c r="CE2" s="17" t="s">
+      <c r="AP2" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:83" s="17" customFormat="1" ht="12.75">
+    <row r="3" spans="2:42" s="17" customFormat="1" ht="12.75">
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
@@ -3880,19 +3900,8 @@
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
-      <c r="AK3" s="1"/>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="1"/>
-      <c r="AN3" s="1"/>
-      <c r="AO3" s="1"/>
-      <c r="AP3" s="1"/>
-      <c r="AQ3" s="1"/>
-      <c r="AR3" s="1"/>
-      <c r="AS3" s="1"/>
-      <c r="AT3" s="1"/>
-      <c r="AU3" s="1"/>
-    </row>
-    <row r="4" spans="2:83" s="18" customFormat="1">
+    </row>
+    <row r="4" spans="2:42" s="18" customFormat="1">
       <c r="B4" s="18" t="s">
         <v>8</v>
       </c>
@@ -3906,22 +3915,11 @@
       <c r="AH4" s="19"/>
       <c r="AI4" s="19"/>
       <c r="AJ4" s="19"/>
-      <c r="AK4" s="19"/>
-      <c r="AL4" s="19"/>
-      <c r="AM4" s="19"/>
-      <c r="AN4" s="19"/>
-      <c r="AO4" s="19"/>
-      <c r="AP4" s="19"/>
-      <c r="AQ4" s="19"/>
-      <c r="AR4" s="19"/>
-      <c r="AS4" s="19"/>
-      <c r="AT4" s="19"/>
-      <c r="AU4" s="19"/>
-      <c r="CE4" s="18" t="s">
+      <c r="AP4" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:83" s="18" customFormat="1">
+    <row r="5" spans="2:42" s="18" customFormat="1">
       <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
@@ -3935,19 +3933,8 @@
       <c r="AH5" s="19"/>
       <c r="AI5" s="19"/>
       <c r="AJ5" s="19"/>
-      <c r="AK5" s="19"/>
-      <c r="AL5" s="19"/>
-      <c r="AM5" s="19"/>
-      <c r="AN5" s="19"/>
-      <c r="AO5" s="19"/>
-      <c r="AP5" s="19"/>
-      <c r="AQ5" s="19"/>
-      <c r="AR5" s="19"/>
-      <c r="AS5" s="19"/>
-      <c r="AT5" s="19"/>
-      <c r="AU5" s="19"/>
-    </row>
-    <row r="8" spans="2:83">
+    </row>
+    <row r="8" spans="2:42">
       <c r="B8" s="27" t="s">
         <v>20</v>
       </c>
@@ -3983,11 +3970,11 @@
       <c r="AG8" s="24"/>
       <c r="AH8" s="24"/>
       <c r="AI8" s="24"/>
-      <c r="CE8" s="57" t="s">
+      <c r="AP8" s="57" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:83">
+    <row r="9" spans="2:42">
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -4018,7 +4005,7 @@
       <c r="AD9" s="24"/>
       <c r="AE9" s="24"/>
     </row>
-    <row r="10" spans="2:83">
+    <row r="10" spans="2:42">
       <c r="B10" s="29" t="s">
         <v>19</v>
       </c>
@@ -4031,18 +4018,18 @@
       <c r="AD10" s="24"/>
       <c r="AE10" s="24"/>
     </row>
-    <row r="11" spans="2:83">
+    <row r="11" spans="2:42">
       <c r="B11" s="29" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:83">
+    <row r="12" spans="2:42">
       <c r="B12" s="23"/>
     </row>
-    <row r="13" spans="2:83" ht="14.25" thickBot="1">
+    <row r="13" spans="2:42" ht="14.25" thickBot="1">
       <c r="B13" s="23"/>
     </row>
-    <row r="14" spans="2:83">
+    <row r="14" spans="2:42">
       <c r="B14" s="23"/>
       <c r="D14" s="82"/>
       <c r="E14" s="83"/>
@@ -4076,7 +4063,7 @@
       <c r="AG14" s="85"/>
       <c r="AH14" s="86"/>
     </row>
-    <row r="15" spans="2:83">
+    <row r="15" spans="2:42">
       <c r="B15" s="25"/>
       <c r="D15" s="87"/>
       <c r="E15" s="61"/>
@@ -4110,7 +4097,7 @@
       <c r="AG15" s="61"/>
       <c r="AH15" s="88"/>
     </row>
-    <row r="16" spans="2:83" ht="14.25" thickBot="1">
+    <row r="16" spans="2:42" ht="14.25" thickBot="1">
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
       <c r="D16" s="87"/>
@@ -5192,7 +5179,7 @@
       <c r="AG48" s="61"/>
       <c r="AH48" s="73"/>
     </row>
-    <row r="49" spans="2:34">
+    <row r="49" spans="2:42">
       <c r="D49" s="74"/>
       <c r="E49" s="61"/>
       <c r="F49" s="61"/>
@@ -5225,7 +5212,7 @@
       <c r="AG49" s="61"/>
       <c r="AH49" s="73"/>
     </row>
-    <row r="50" spans="2:34">
+    <row r="50" spans="2:42">
       <c r="D50" s="74"/>
       <c r="E50" s="61"/>
       <c r="F50" s="61"/>
@@ -5258,7 +5245,7 @@
       <c r="AG50" s="61"/>
       <c r="AH50" s="73"/>
     </row>
-    <row r="51" spans="2:34">
+    <row r="51" spans="2:42">
       <c r="D51" s="74"/>
       <c r="E51" s="61"/>
       <c r="F51" s="61"/>
@@ -5291,7 +5278,7 @@
       <c r="AG51" s="61"/>
       <c r="AH51" s="73"/>
     </row>
-    <row r="52" spans="2:34">
+    <row r="52" spans="2:42">
       <c r="D52" s="74"/>
       <c r="E52" s="61"/>
       <c r="F52" s="61"/>
@@ -5324,7 +5311,7 @@
       <c r="AG52" s="61"/>
       <c r="AH52" s="73"/>
     </row>
-    <row r="53" spans="2:34">
+    <row r="53" spans="2:42">
       <c r="D53" s="74"/>
       <c r="E53" s="61"/>
       <c r="F53" s="61"/>
@@ -5357,7 +5344,7 @@
       <c r="AG53" s="61"/>
       <c r="AH53" s="73"/>
     </row>
-    <row r="54" spans="2:34">
+    <row r="54" spans="2:42">
       <c r="D54" s="74"/>
       <c r="E54" s="61"/>
       <c r="F54" s="61"/>
@@ -5390,7 +5377,7 @@
       <c r="AG54" s="61"/>
       <c r="AH54" s="73"/>
     </row>
-    <row r="55" spans="2:34">
+    <row r="55" spans="2:42">
       <c r="B55" s="23"/>
       <c r="C55" s="23"/>
       <c r="D55" s="75"/>
@@ -5425,7 +5412,7 @@
       <c r="AG55" s="65"/>
       <c r="AH55" s="76"/>
     </row>
-    <row r="56" spans="2:34" ht="14.25" thickBot="1">
+    <row r="56" spans="2:42" ht="14.25" thickBot="1">
       <c r="B56" s="23"/>
       <c r="C56" s="23"/>
       <c r="D56" s="77"/>
@@ -5462,7 +5449,7 @@
       <c r="AG56" s="80"/>
       <c r="AH56" s="81"/>
     </row>
-    <row r="57" spans="2:34">
+    <row r="57" spans="2:42">
       <c r="B57" s="24"/>
       <c r="C57" s="24"/>
       <c r="D57" s="24"/>
@@ -5493,8 +5480,11 @@
       <c r="AC57" s="24"/>
       <c r="AD57" s="24"/>
       <c r="AE57" s="24"/>
-    </row>
-    <row r="58" spans="2:34">
+      <c r="AP57" s="57" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="2:42">
       <c r="B58" s="24"/>
       <c r="C58" s="24"/>
       <c r="D58" s="24"/>
@@ -5526,7 +5516,7 @@
       <c r="AD58" s="24"/>
       <c r="AE58" s="24"/>
     </row>
-    <row r="59" spans="2:34">
+    <row r="59" spans="2:42">
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
       <c r="D59" s="24"/>
@@ -5558,7 +5548,7 @@
       <c r="AD59" s="24"/>
       <c r="AE59" s="24"/>
     </row>
-    <row r="60" spans="2:34">
+    <row r="60" spans="2:42">
       <c r="B60" s="98" t="s">
         <v>67</v>
       </c>
@@ -5592,7 +5582,7 @@
       <c r="AD60" s="24"/>
       <c r="AE60" s="24"/>
     </row>
-    <row r="61" spans="2:34">
+    <row r="61" spans="2:42">
       <c r="B61" s="24"/>
       <c r="C61" s="24"/>
       <c r="D61" s="24"/>
@@ -5624,7 +5614,7 @@
       <c r="AD61" s="24"/>
       <c r="AE61" s="24"/>
     </row>
-    <row r="62" spans="2:34">
+    <row r="62" spans="2:42">
       <c r="B62" s="26" t="s">
         <v>66</v>
       </c>
@@ -5658,12 +5648,12 @@
       <c r="AD62" s="24"/>
       <c r="AE62" s="24"/>
     </row>
-    <row r="63" spans="2:34">
+    <row r="63" spans="2:42">
       <c r="B63" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="2:34">
+    <row r="64" spans="2:42">
       <c r="B64" s="20" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
2019.07.23.Tus. 00:54 Git and SVN Information
</commit_message>
<xml_diff>
--- a/GitGitHubSVN.xlsx
+++ b/GitGitHubSVN.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="14730" windowHeight="8940" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="14730" windowHeight="8940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="History" sheetId="1" r:id="rId1"/>
     <sheet name="Git" sheetId="2" r:id="rId2"/>
+    <sheet name="SVN" sheetId="3" r:id="rId3"/>
+    <sheet name="Sample" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t>작업이력</t>
     <phoneticPr fontId="6" type="noConversion"/>
@@ -102,10 +105,6 @@
   </si>
   <si>
     <t>git push origin +master</t>
-  </si>
-  <si>
-    <t>Git 실습하기</t>
-    <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -470,12 +469,112 @@
     <t>GitHub 계정을 만들고, 파일을 올린다. (Push) - 크롬에서 Octotree 를 설치하면 왼쪽에 탐색기처럼 나타난다.</t>
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
+  <si>
+    <t>Git 실습하기 - GitHub 계정 및 README.md 모양내기</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Git 실습하기 - Git Client 설치 및 add, commit, push 연습</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Git 윈도우버전 다운 및 설치하기 - Windows용 : https://git-scm.com/download/win</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Git Bash 화면에서 git init 부터 push 까지 실행 (중간에 로그인창 나타나며, 앞서 GitHub 에 신규등록한 계정으로 로그인)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인을 하면 push 명령어를 통해 원격저장소(remote repository) 로 폴더, 파일 전송된다.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   ▶▶ [Downloads] ▶▶ OS 버전에 맞는 설치 파일 다운로드 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ▶▶ 다운로드 받은 설치 파일 클릭 ▶▶ [NEXT]로 계속 진행 ▶▶ 바탕화면에 생성된 [Git Bash] 클릭하면 Shell이 뜸</t>
+  </si>
+  <si>
+    <t>git 홈페이지 :  https://git-scm.com/download/win  (Windows용)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Git 설치 - Git client 버전 설치</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>GitHub 홈페이지</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ▶▶ [Sign up for GitHub] 클릭 ▶▶ 이름, 이메일, 패스워드 입력</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ▶▶ [Create an account] ▶▶ 무료(공개) 버전 또는 유료(개인 저장소) 선택 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ▶▶ [Continue] ▶▶ 설문 답변 또는 [skip this step] ▶▶ [Start a Project] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ▶▶ 이메일 인증 안내 화면 ▶▶ 메일의 [Verify email address] 클릭 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   ▶▶ [Start a Project]</t>
+  </si>
+  <si>
+    <t>GitHub 설치 (GitHub 가입) : https://github.com/</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVN (Visual SVN Server, 윈도우버전)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반적으로 Linux 에서 SVN 을 사용하였지만, 윈도우용 SVN Server 도 추천한다.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVN 설치 - https://www.visualsvn.com/</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>무료사용! 15 user Community 버전의 경우 무료로 사용할 수 있다.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>다운로드 받아서 설치해보자.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제 사용하고 있는 화면 사례 (Logging 기능 등을 이용하면 운영체제에서 로그를 남길 수는 있으나, 유료버전이 되므로 기본값 disable 상태를 유지한다)</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVN 클라이언트 설치</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>Visaul SVN 설치 Snapshot</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVN 설치 및 주요기능 확인</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>SVN 의 경우 Commit, Update 를 통해 SVN 서버에 파일을 올리고, 다운받는 것으로만 생각했는데,</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>최근 Git 과 비슷한 형태로 확인할 수 있다.</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="16">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +697,30 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFC00000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
       <color rgb="FFC00000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -1187,7 +1310,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1483,6 +1606,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2012,14 +2144,14 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>264583</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>116375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>127333</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>32083</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>148458</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2036,7 +2168,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13980583" y="1492250"/>
+          <a:off x="10837333" y="2815125"/>
           <a:ext cx="720000" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2050,14 +2182,14 @@
     <xdr:from>
       <xdr:col>41</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>116375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>74</xdr:col>
       <xdr:colOff>246441</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>28667</xdr:rowOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>155626</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2074,7 +2206,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14859000" y="1492250"/>
+          <a:off x="11715750" y="2815125"/>
           <a:ext cx="9676191" cy="7733334"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3108,14 +3240,14 @@
     <xdr:from>
       <xdr:col>41</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>169290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>76</xdr:col>
       <xdr:colOff>189227</xdr:colOff>
-      <xdr:row>130</xdr:row>
-      <xdr:rowOff>112763</xdr:rowOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>112720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3132,8 +3264,414 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11715750" y="9884833"/>
+          <a:off x="11715750" y="11239457"/>
           <a:ext cx="10190477" cy="12304763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>89</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>10535</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>121</xdr:col>
+      <xdr:colOff>36953</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>156642</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="그림 34" descr="598_github_client.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25431750" y="2878618"/>
+          <a:ext cx="9180953" cy="8009524"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>89</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>158708</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>105</xdr:col>
+      <xdr:colOff>180381</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>119089</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="그림 35" descr="600_github_client.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25431750" y="11059541"/>
+          <a:ext cx="4752381" cy="3685715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>89</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>10546</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>118</xdr:col>
+      <xdr:colOff>198965</xdr:colOff>
+      <xdr:row>192</xdr:row>
+      <xdr:rowOff>31690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="그림 36" descr="603_github_practice.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25431750" y="15483379"/>
+          <a:ext cx="8485715" cy="17123811"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>89</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>196</xdr:row>
+      <xdr:rowOff>10546</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>118</xdr:col>
+      <xdr:colOff>198965</xdr:colOff>
+      <xdr:row>297</xdr:row>
+      <xdr:rowOff>31690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="그림 37" descr="604_github_practice.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="25431750" y="33263379"/>
+          <a:ext cx="8485715" cy="17123811"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>264583</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>52921</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>127333</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>85004</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="그림 38" descr="63_git_logo.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10837333" y="3619504"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>275155</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>8610</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1" descr="603_visual_svn.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="1743075"/>
+          <a:ext cx="8561905" cy="7323810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>27433</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>56118</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="그림 2" descr="604_visual_svn_license.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="9696450"/>
+          <a:ext cx="9142858" cy="8257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>27433</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>27543</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="그림 3" descr="605_visual_svn_download.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="18507075"/>
+          <a:ext cx="9142858" cy="8257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>179</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>103623</xdr:colOff>
+      <xdr:row>228</xdr:row>
+      <xdr:rowOff>132401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="그림 4" descr="606_visual_svn_info.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="27346275"/>
+          <a:ext cx="9219048" cy="7600001"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>79</xdr:col>
+      <xdr:colOff>65390</xdr:colOff>
+      <xdr:row>526</xdr:row>
+      <xdr:rowOff>114024</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="그림 7" descr="607_visual_svn_info.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11601450" y="1895475"/>
+          <a:ext cx="10285715" cy="78447624"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3528,10 +4066,10 @@
         <v>2</v>
       </c>
       <c r="C7" s="96" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="97" t="s">
         <v>42</v>
-      </c>
-      <c r="D7" s="97" t="s">
-        <v>43</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>5</v>
@@ -3846,12 +4384,12 @@
   <sheetPr>
     <tabColor rgb="FFFFFFCC"/>
   </sheetPr>
-  <dimension ref="B1:AP136"/>
+  <dimension ref="B1:CL195"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" topLeftCell="AD1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AM30" sqref="AM30"/>
-      <selection pane="bottomLeft" activeCell="AP58" sqref="AP58"/>
+      <selection pane="bottomLeft" activeCell="AM30" sqref="AM30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.75" defaultRowHeight="13.5"/>
@@ -3859,7 +4397,7 @@
     <col min="1" max="16384" width="3.75" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" s="17" customFormat="1" ht="12.75">
+    <row r="1" spans="2:90" s="17" customFormat="1" ht="12.75">
       <c r="AA1" s="1"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
@@ -3871,9 +4409,9 @@
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
     </row>
-    <row r="2" spans="2:42" s="17" customFormat="1" ht="12.75">
+    <row r="2" spans="2:90" s="17" customFormat="1" ht="12.75">
       <c r="B2" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
@@ -3886,10 +4424,13 @@
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1"/>
       <c r="AP2" s="17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="2:42" s="17" customFormat="1" ht="12.75">
+        <v>84</v>
+      </c>
+      <c r="CL2" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="2:90" s="17" customFormat="1" ht="12.75">
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
@@ -3901,7 +4442,7 @@
       <c r="AI3" s="1"/>
       <c r="AJ3" s="1"/>
     </row>
-    <row r="4" spans="2:42" s="18" customFormat="1">
+    <row r="4" spans="2:90" s="18" customFormat="1">
       <c r="B4" s="18" t="s">
         <v>8</v>
       </c>
@@ -3916,10 +4457,10 @@
       <c r="AI4" s="19"/>
       <c r="AJ4" s="19"/>
       <c r="AP4" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="2:42" s="18" customFormat="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:90" s="18" customFormat="1">
       <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
@@ -3934,9 +4475,9 @@
       <c r="AI5" s="19"/>
       <c r="AJ5" s="19"/>
     </row>
-    <row r="8" spans="2:42">
+    <row r="8" spans="2:90">
       <c r="B8" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
@@ -3971,10 +4512,13 @@
       <c r="AH8" s="24"/>
       <c r="AI8" s="24"/>
       <c r="AP8" s="57" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="2:42">
+        <v>99</v>
+      </c>
+      <c r="CL8" s="57" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="2:90">
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -4004,10 +4548,16 @@
       <c r="AC9" s="23"/>
       <c r="AD9" s="24"/>
       <c r="AE9" s="24"/>
-    </row>
-    <row r="10" spans="2:42">
+      <c r="AP9" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="CL9" s="99" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="2:90">
       <c r="B10" s="29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="23"/>
       <c r="Y10" s="23"/>
@@ -4017,19 +4567,37 @@
       <c r="AC10" s="23"/>
       <c r="AD10" s="24"/>
       <c r="AE10" s="24"/>
-    </row>
-    <row r="11" spans="2:42">
+      <c r="AP10" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="CL10" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="2:90">
       <c r="B11" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:42">
+        <v>17</v>
+      </c>
+      <c r="AP11" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="CL11" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="2:90">
       <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="2:42" ht="14.25" thickBot="1">
+      <c r="AP12" s="20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="2:90" ht="14.25" thickBot="1">
       <c r="B13" s="23"/>
-    </row>
-    <row r="14" spans="2:42">
+      <c r="AP13" s="20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="2:90">
       <c r="B14" s="23"/>
       <c r="D14" s="82"/>
       <c r="E14" s="83"/>
@@ -4062,8 +4630,11 @@
       <c r="AF14" s="85"/>
       <c r="AG14" s="85"/>
       <c r="AH14" s="86"/>
-    </row>
-    <row r="15" spans="2:42">
+      <c r="AP14" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="2:90">
       <c r="B15" s="25"/>
       <c r="D15" s="87"/>
       <c r="E15" s="61"/>
@@ -4097,11 +4668,17 @@
       <c r="AG15" s="61"/>
       <c r="AH15" s="88"/>
     </row>
-    <row r="16" spans="2:42" ht="14.25" thickBot="1">
+    <row r="16" spans="2:90" ht="14.25" thickBot="1">
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
       <c r="D16" s="87"/>
       <c r="AH16" s="88"/>
+      <c r="AP16" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="CL16" s="57" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="17" spans="2:34">
       <c r="B17" s="23"/>
@@ -4145,43 +4722,43 @@
       <c r="E18" s="35"/>
       <c r="F18" s="30"/>
       <c r="G18" s="52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H18" s="31"/>
       <c r="I18" s="36"/>
       <c r="J18" s="58"/>
       <c r="K18" s="60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L18" s="59"/>
       <c r="M18" s="44"/>
       <c r="N18" s="45"/>
       <c r="O18" s="53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P18" s="47"/>
       <c r="Q18" s="48"/>
       <c r="R18" s="58"/>
       <c r="S18" s="60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T18" s="59"/>
       <c r="U18" s="35"/>
       <c r="V18" s="30"/>
       <c r="W18" s="54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X18" s="31"/>
       <c r="Y18" s="36"/>
       <c r="Z18" s="58"/>
       <c r="AA18" s="60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AB18" s="59"/>
       <c r="AC18" s="35"/>
       <c r="AD18" s="30"/>
       <c r="AE18" s="54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AF18" s="31"/>
       <c r="AG18" s="36"/>
@@ -4194,43 +4771,43 @@
       <c r="E19" s="35"/>
       <c r="F19" s="30"/>
       <c r="G19" s="40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" s="31"/>
       <c r="I19" s="36"/>
       <c r="J19" s="35"/>
       <c r="K19" s="55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L19" s="36"/>
       <c r="M19" s="44"/>
       <c r="N19" s="45"/>
       <c r="O19" s="46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P19" s="47"/>
       <c r="Q19" s="48"/>
       <c r="R19" s="31"/>
       <c r="S19" s="66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="T19" s="31"/>
       <c r="U19" s="35"/>
       <c r="V19" s="30"/>
       <c r="W19" s="40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X19" s="31"/>
       <c r="Y19" s="36"/>
       <c r="Z19" s="61"/>
       <c r="AA19" s="55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AB19" s="31"/>
       <c r="AC19" s="35"/>
       <c r="AD19" s="30"/>
       <c r="AE19" s="40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AF19" s="31"/>
       <c r="AG19" s="36"/>
@@ -4243,7 +4820,7 @@
       <c r="E20" s="35"/>
       <c r="F20" s="30"/>
       <c r="G20" s="40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H20" s="31"/>
       <c r="I20" s="36"/>
@@ -4253,7 +4830,7 @@
       <c r="M20" s="44"/>
       <c r="N20" s="45"/>
       <c r="O20" s="46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P20" s="47"/>
       <c r="Q20" s="48"/>
@@ -4434,7 +5011,7 @@
       <c r="Q25" s="92"/>
       <c r="R25" s="92"/>
       <c r="S25" s="93" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="T25" s="92"/>
       <c r="U25" s="92"/>
@@ -4776,7 +5353,7 @@
       <c r="E37" s="35"/>
       <c r="F37" s="30"/>
       <c r="G37" s="54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H37" s="31"/>
       <c r="I37" s="36"/>
@@ -4786,7 +5363,7 @@
       <c r="M37" s="44"/>
       <c r="N37" s="45"/>
       <c r="O37" s="53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P37" s="47"/>
       <c r="Q37" s="48"/>
@@ -4796,7 +5373,7 @@
       <c r="U37" s="35"/>
       <c r="V37" s="30"/>
       <c r="W37" s="54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="X37" s="31"/>
       <c r="Y37" s="36"/>
@@ -4806,7 +5383,7 @@
       <c r="AC37" s="35"/>
       <c r="AD37" s="30"/>
       <c r="AE37" s="54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AF37" s="31"/>
       <c r="AG37" s="36"/>
@@ -4833,7 +5410,7 @@
       <c r="U38" s="35"/>
       <c r="V38" s="30"/>
       <c r="W38" s="40" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X38" s="31"/>
       <c r="Y38" s="36"/>
@@ -4843,7 +5420,7 @@
       <c r="AC38" s="35"/>
       <c r="AD38" s="30"/>
       <c r="AE38" s="40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AF38" s="31"/>
       <c r="AG38" s="36"/>
@@ -5179,7 +5756,7 @@
       <c r="AG48" s="61"/>
       <c r="AH48" s="73"/>
     </row>
-    <row r="49" spans="2:42">
+    <row r="49" spans="2:34">
       <c r="D49" s="74"/>
       <c r="E49" s="61"/>
       <c r="F49" s="61"/>
@@ -5212,7 +5789,7 @@
       <c r="AG49" s="61"/>
       <c r="AH49" s="73"/>
     </row>
-    <row r="50" spans="2:42">
+    <row r="50" spans="2:34">
       <c r="D50" s="74"/>
       <c r="E50" s="61"/>
       <c r="F50" s="61"/>
@@ -5245,7 +5822,7 @@
       <c r="AG50" s="61"/>
       <c r="AH50" s="73"/>
     </row>
-    <row r="51" spans="2:42">
+    <row r="51" spans="2:34">
       <c r="D51" s="74"/>
       <c r="E51" s="61"/>
       <c r="F51" s="61"/>
@@ -5278,7 +5855,7 @@
       <c r="AG51" s="61"/>
       <c r="AH51" s="73"/>
     </row>
-    <row r="52" spans="2:42">
+    <row r="52" spans="2:34">
       <c r="D52" s="74"/>
       <c r="E52" s="61"/>
       <c r="F52" s="61"/>
@@ -5311,7 +5888,7 @@
       <c r="AG52" s="61"/>
       <c r="AH52" s="73"/>
     </row>
-    <row r="53" spans="2:42">
+    <row r="53" spans="2:34">
       <c r="D53" s="74"/>
       <c r="E53" s="61"/>
       <c r="F53" s="61"/>
@@ -5344,7 +5921,7 @@
       <c r="AG53" s="61"/>
       <c r="AH53" s="73"/>
     </row>
-    <row r="54" spans="2:42">
+    <row r="54" spans="2:34">
       <c r="D54" s="74"/>
       <c r="E54" s="61"/>
       <c r="F54" s="61"/>
@@ -5377,7 +5954,7 @@
       <c r="AG54" s="61"/>
       <c r="AH54" s="73"/>
     </row>
-    <row r="55" spans="2:42">
+    <row r="55" spans="2:34">
       <c r="B55" s="23"/>
       <c r="C55" s="23"/>
       <c r="D55" s="75"/>
@@ -5412,7 +5989,7 @@
       <c r="AG55" s="65"/>
       <c r="AH55" s="76"/>
     </row>
-    <row r="56" spans="2:42" ht="14.25" thickBot="1">
+    <row r="56" spans="2:34" ht="14.25" thickBot="1">
       <c r="B56" s="23"/>
       <c r="C56" s="23"/>
       <c r="D56" s="77"/>
@@ -5431,7 +6008,7 @@
       <c r="Q56" s="78"/>
       <c r="R56" s="78"/>
       <c r="S56" s="79" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T56" s="78"/>
       <c r="U56" s="78"/>
@@ -5449,7 +6026,7 @@
       <c r="AG56" s="80"/>
       <c r="AH56" s="81"/>
     </row>
-    <row r="57" spans="2:42">
+    <row r="57" spans="2:34">
       <c r="B57" s="24"/>
       <c r="C57" s="24"/>
       <c r="D57" s="24"/>
@@ -5480,11 +6057,8 @@
       <c r="AC57" s="24"/>
       <c r="AD57" s="24"/>
       <c r="AE57" s="24"/>
-      <c r="AP57" s="57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="2:42">
+    </row>
+    <row r="58" spans="2:34">
       <c r="B58" s="24"/>
       <c r="C58" s="24"/>
       <c r="D58" s="24"/>
@@ -5516,7 +6090,7 @@
       <c r="AD58" s="24"/>
       <c r="AE58" s="24"/>
     </row>
-    <row r="59" spans="2:42">
+    <row r="59" spans="2:34">
       <c r="B59" s="24"/>
       <c r="C59" s="24"/>
       <c r="D59" s="24"/>
@@ -5548,9 +6122,9 @@
       <c r="AD59" s="24"/>
       <c r="AE59" s="24"/>
     </row>
-    <row r="60" spans="2:42">
+    <row r="60" spans="2:34">
       <c r="B60" s="98" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C60" s="24"/>
       <c r="D60" s="24"/>
@@ -5582,7 +6156,7 @@
       <c r="AD60" s="24"/>
       <c r="AE60" s="24"/>
     </row>
-    <row r="61" spans="2:42">
+    <row r="61" spans="2:34">
       <c r="B61" s="24"/>
       <c r="C61" s="24"/>
       <c r="D61" s="24"/>
@@ -5614,9 +6188,9 @@
       <c r="AD61" s="24"/>
       <c r="AE61" s="24"/>
     </row>
-    <row r="62" spans="2:42">
+    <row r="62" spans="2:34">
       <c r="B62" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" s="24"/>
       <c r="D62" s="24"/>
@@ -5648,224 +6222,237 @@
       <c r="AD62" s="24"/>
       <c r="AE62" s="24"/>
     </row>
-    <row r="63" spans="2:42">
+    <row r="63" spans="2:34">
       <c r="B63" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="2:42">
+    <row r="64" spans="2:34">
       <c r="B64" s="20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="2:2">
+    <row r="65" spans="2:42">
+      <c r="AP65" s="57" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="66" spans="2:42">
       <c r="B66" s="22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="2:42">
       <c r="B67" s="20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="2:2">
+    <row r="69" spans="2:42">
       <c r="B69" s="22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="2:42">
       <c r="B70" s="20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="2:2">
+    <row r="71" spans="2:42">
       <c r="B71" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="2:2">
+    <row r="72" spans="2:42">
       <c r="B72" s="20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="2:2">
+    <row r="73" spans="2:42">
       <c r="B73" s="20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="77" spans="2:2">
+    <row r="77" spans="2:42">
       <c r="B77" s="57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="2:42">
+      <c r="B79" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="81" spans="2:90">
+      <c r="C81" s="56" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="79" spans="2:2">
-      <c r="B79" s="22" t="s">
+    <row r="82" spans="2:90">
+      <c r="C82" s="56" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="83" spans="2:90">
+      <c r="C83" s="56" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="2:90">
+      <c r="B85" s="22" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="2:3">
-      <c r="C81" s="56" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="82" spans="2:3">
-      <c r="C82" s="56" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="83" spans="2:3">
-      <c r="C83" s="56" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="85" spans="2:3">
-      <c r="B85" s="22" t="s">
+    <row r="87" spans="2:90">
+      <c r="C87" s="56" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="2:3">
-      <c r="C87" s="56" t="s">
+    <row r="88" spans="2:90">
+      <c r="C88" s="20" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="88" spans="2:3">
-      <c r="C88" s="20" t="s">
+    <row r="90" spans="2:90">
+      <c r="B90" s="22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="90" spans="2:3">
-      <c r="B90" s="22" t="s">
+      <c r="CL90" s="57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92" spans="2:90">
+      <c r="C92" s="56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="92" spans="2:3">
-      <c r="C92" s="56" t="s">
+    <row r="93" spans="2:90">
+      <c r="C93" s="56" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="93" spans="2:3">
-      <c r="C93" s="56" t="s">
+    <row r="94" spans="2:90">
+      <c r="C94" s="56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="94" spans="2:3">
-      <c r="C94" s="56" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="96" spans="2:3">
+    <row r="96" spans="2:90">
       <c r="B96" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="98" spans="2:3">
       <c r="C98" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="99" spans="2:3">
       <c r="C99" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="100" spans="2:3">
       <c r="C100" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="102" spans="2:3">
       <c r="B102" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="104" spans="2:3">
       <c r="C104" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="105" spans="2:3">
       <c r="C105" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="108" spans="2:3">
       <c r="B108" s="57" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="110" spans="2:3">
       <c r="B110" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="111" spans="2:3">
       <c r="B111" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="113" spans="2:3">
       <c r="B113" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="114" spans="2:3">
       <c r="B114" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="115" spans="2:3">
       <c r="B115" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="119" spans="2:3">
       <c r="B119" s="57" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="121" spans="2:3">
       <c r="B121" s="22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="123" spans="2:3">
       <c r="C123" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="125" spans="2:3">
       <c r="B125" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="127" spans="2:3">
       <c r="C127" s="20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="129" spans="2:3">
       <c r="B129" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="131" spans="2:3">
       <c r="C131" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="132" spans="2:3">
       <c r="C132" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="134" spans="2:3">
       <c r="B134" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="136" spans="2:3">
       <c r="C136" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="195" spans="90:90">
+      <c r="CL195" s="57" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -5875,4 +6462,103 @@
   <drawing r:id="rId2"/>
   <picture r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B1:CA178"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AO392" sqref="AO392"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="16384" width="3.625" style="100"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:79" s="1" customFormat="1" ht="12.75"/>
+    <row r="2" spans="2:79" s="1" customFormat="1" ht="12.75">
+      <c r="B2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="CA2" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="2:79" s="1" customFormat="1" ht="12.75"/>
+    <row r="4" spans="2:79" s="19" customFormat="1" ht="13.5"/>
+    <row r="5" spans="2:79" s="19" customFormat="1" ht="13.5"/>
+    <row r="8" spans="2:79">
+      <c r="B8" s="101" t="s">
+        <v>102</v>
+      </c>
+      <c r="AQ8" s="101" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="2:79">
+      <c r="B10" s="100" t="s">
+        <v>101</v>
+      </c>
+      <c r="AQ10" s="100" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="2:79">
+      <c r="AQ11" s="100" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="101" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" s="101" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2">
+      <c r="B178" s="101" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <picture r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="12"/>
+  <cols>
+    <col min="1" max="16384" width="3.625" style="100"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="12.75"/>
+    <row r="2" s="1" customFormat="1" ht="12.75"/>
+    <row r="3" s="1" customFormat="1" ht="12.75"/>
+    <row r="4" s="19" customFormat="1" ht="13.5"/>
+    <row r="5" s="19" customFormat="1" ht="13.5"/>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>